<commit_message>
updated the opengraph image
</commit_message>
<xml_diff>
--- a/public/Website and social media content (1).xlsx
+++ b/public/Website and social media content (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadic\Dropbox\My projects\myJamii\Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dessie/Documents/Abdul Majid Njozi/development/my-jamii-website/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC751591-0FF6-44DA-AE2E-D88ADC9BF8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144017C7-C5B5-524E-8209-D9845A9BFF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{74514E31-8705-4D36-B854-03CEBB69E461}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30220" windowHeight="17200" xr2:uid="{74514E31-8705-4D36-B854-03CEBB69E461}"/>
   </bookViews>
   <sheets>
     <sheet name="Website content" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1086,24 +1084,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1119,6 +1099,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1128,10 +1123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1470,556 +1468,556 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BC9586-236A-424A-9420-CCD24EB43262}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="4"/>
+    <col min="6" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="17" t="s">
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="17" t="s">
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="17" t="s">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="17" t="s">
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="17" t="s">
+    <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="11" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="17" t="s">
+    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="11" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="17" t="s">
+    <row r="11" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="11" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="17" t="s">
+    <row r="12" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="17" t="s">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="17" t="s">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="11" t="s">
         <v>52</v>
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="17" t="s">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="11" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="17" t="s">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="11" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="17" t="s">
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="17" t="s">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="17" t="s">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="17" t="s">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="11" t="s">
         <v>69</v>
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="17" t="s">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="11" t="s">
         <v>70</v>
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="17" t="s">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="11" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="17" t="s">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="11" t="s">
         <v>72</v>
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="17" t="s">
+    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="11" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="17" t="s">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="11" t="s">
         <v>85</v>
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="17" t="s">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="11" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="17" t="s">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="11" t="s">
         <v>87</v>
       </c>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="17" t="s">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="11" t="s">
         <v>88</v>
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="17" t="s">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="11" t="s">
         <v>89</v>
       </c>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="17" t="s">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="11" t="s">
         <v>90</v>
       </c>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="17" t="s">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="11" t="s">
         <v>82</v>
       </c>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="17" t="s">
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="11" t="s">
         <v>92</v>
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="17" t="s">
+    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="11" t="s">
         <v>93</v>
       </c>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="11" t="s">
         <v>95</v>
       </c>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="17" t="s">
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="11" t="s">
         <v>96</v>
       </c>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="17" t="s">
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="11" t="s">
         <v>98</v>
       </c>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2028,30 +2026,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A22:A27"/>
     <mergeCell ref="C28:C37"/>
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="A28:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2061,199 +2059,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4D5A8F-99DF-4EDE-A94E-8CCED2EF908C}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="16.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="17" t="s">
         <v>106</v>
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="22" t="s">
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="22" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="16" t="s">
         <v>111</v>
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="16" t="s">
         <v>110</v>
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="16" t="s">
         <v>112</v>
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="16" t="s">
         <v>119</v>
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
-      <c r="B8" s="22" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
+      <c r="B8" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>113</v>
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+      <c r="B9" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="16" t="s">
         <v>115</v>
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
-      <c r="B10" s="22" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="22" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>118</v>
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="25"/>
+      <c r="B12" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="16" t="s">
         <v>121</v>
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="22" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="16" t="s">
         <v>122</v>
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="27"/>
+      <c r="B15" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="16" t="s">
         <v>123</v>
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
-      <c r="B16" s="22" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="16" t="s">
         <v>124</v>
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="22" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="16" t="s">
         <v>125</v>
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>